<commit_message>
Added daily and monthly reports
</commit_message>
<xml_diff>
--- a/uploads/Fe.xlsx
+++ b/uploads/Fe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kde docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF536C4-4C33-471B-9C23-D7980FA253F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799B39FC-9114-4983-A497-B21565971A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FA3CA76D-9751-48DC-BF4C-57F928EA1419}"/>
+    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="12624" xr2:uid="{FA3CA76D-9751-48DC-BF4C-57F928EA1419}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="55">
   <si>
     <t>Dnyaneshwar</t>
   </si>
@@ -127,9 +127,6 @@
     <t>payscale_per_hour</t>
   </si>
   <si>
-    <t>ACSED45</t>
-  </si>
-  <si>
     <t>Aman Shaikh</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
     <t>abc.com</t>
   </si>
   <si>
-    <t>PH - Ladies Standard</t>
-  </si>
-  <si>
     <t>Nanded Bank</t>
   </si>
   <si>
@@ -169,25 +163,40 @@
     <t>Other</t>
   </si>
   <si>
-    <t>Daily</t>
-  </si>
-  <si>
     <t>ACSED46</t>
   </si>
   <si>
     <t>ACSED47</t>
   </si>
   <si>
-    <t>Vinayak Gaikwad</t>
-  </si>
-  <si>
     <t>Sankket sonawane</t>
   </si>
   <si>
-    <t>Karan Shinde</t>
-  </si>
-  <si>
-    <t>CDCSED512</t>
+    <t>Amaan Shaikh</t>
+  </si>
+  <si>
+    <t>Asha Kaale</t>
+  </si>
+  <si>
+    <t>ACSED10</t>
+  </si>
+  <si>
+    <t>PH ladies - standard</t>
+  </si>
+  <si>
+    <t>Per Day</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>PH Bengal Boys Supervisor</t>
+  </si>
+  <si>
+    <t>Ajit Shinde</t>
+  </si>
+  <si>
+    <t>ACSED11</t>
   </si>
 </sst>
 </file>
@@ -566,7 +575,7 @@
   <dimension ref="A1:AD5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -697,13 +706,13 @@
     </row>
     <row r="2" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B2" s="3">
-        <v>75964565</v>
+        <v>2001</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="5">
         <v>44486</v>
@@ -712,25 +721,25 @@
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="H2" s="3">
         <v>8574968574</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="K2" s="3">
         <v>10</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M2" s="3">
         <v>2</v>
@@ -739,49 +748,49 @@
         <v>748596415263</v>
       </c>
       <c r="O2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="T2" s="4">
         <v>85749685967</v>
       </c>
       <c r="U2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="Z2" s="3">
         <v>9657690018</v>
       </c>
-      <c r="AA2" s="3">
-        <v>100</v>
+      <c r="AA2" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="AB2" s="3">
         <v>100</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="AD2" s="3">
         <v>100</v>
@@ -789,13 +798,13 @@
     </row>
     <row r="3" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B3" s="3">
-        <v>45964965</v>
+        <v>2002</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D3" s="5">
         <v>44486</v>
@@ -804,25 +813,25 @@
         <v>0</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="H3" s="3">
         <v>8574968574</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="K3" s="3">
         <v>10</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M3" s="3">
         <v>2</v>
@@ -831,49 +840,49 @@
         <v>748596415263</v>
       </c>
       <c r="O3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="T3" s="4">
         <v>85749685967</v>
       </c>
       <c r="U3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="Z3" s="3">
         <v>9657690018</v>
       </c>
-      <c r="AA3" s="3">
-        <v>100</v>
+      <c r="AA3" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="AB3" s="3">
         <v>100</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="AD3" s="3">
         <v>100</v>
@@ -881,13 +890,13 @@
     </row>
     <row r="4" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2003</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B4" s="3">
-        <v>25764565</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="D4" s="5">
         <v>44486</v>
@@ -896,25 +905,25 @@
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="H4" s="3">
         <v>8574968574</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="K4" s="3">
         <v>10</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M4" s="3">
         <v>2</v>
@@ -923,49 +932,49 @@
         <v>748596415263</v>
       </c>
       <c r="O4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="T4" s="4">
         <v>85749685967</v>
       </c>
       <c r="U4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="Z4" s="3">
         <v>9657690018</v>
       </c>
-      <c r="AA4" s="3">
-        <v>100</v>
+      <c r="AA4" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="AB4" s="3">
         <v>100</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="AD4" s="3">
         <v>100</v>
@@ -973,13 +982,13 @@
     </row>
     <row r="5" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B5" s="3">
-        <v>35764565</v>
+        <v>2005</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D5" s="5">
         <v>44486</v>
@@ -988,25 +997,25 @@
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="H5" s="3">
         <v>8574968574</v>
       </c>
       <c r="I5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="K5" s="3">
         <v>10</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M5" s="3">
         <v>2</v>
@@ -1015,49 +1024,49 @@
         <v>748596415263</v>
       </c>
       <c r="O5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S5" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="T5" s="4">
         <v>85749685967</v>
       </c>
       <c r="U5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="V5" s="3" t="s">
+      <c r="Y5" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="W5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="X5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y5" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="Z5" s="3">
         <v>9657690018</v>
       </c>
-      <c r="AA5" s="3">
-        <v>100</v>
+      <c r="AA5" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="AB5" s="3">
         <v>100</v>
       </c>
       <c r="AC5" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="AD5" s="3">
         <v>100</v>

</xml_diff>

<commit_message>
Added admin and supervisors
</commit_message>
<xml_diff>
--- a/uploads/Fe.xlsx
+++ b/uploads/Fe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kde docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232E7F5E-B1C9-4037-B560-5FA8142EC54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E817DA6-CC20-4AEB-8B94-F5FA38786B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="12624" xr2:uid="{FA3CA76D-9751-48DC-BF4C-57F928EA1419}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="56">
   <si>
     <t>Dnyaneshwar</t>
   </si>
@@ -118,15 +118,9 @@
     <t>pay_scale_term</t>
   </si>
   <si>
-    <t>pay_scale</t>
-  </si>
-  <si>
     <t>pay_scale_type</t>
   </si>
   <si>
-    <t>payscale_per_hour</t>
-  </si>
-  <si>
     <t>Sangli</t>
   </si>
   <si>
@@ -194,6 +188,18 @@
   </si>
   <si>
     <t>Krishna Mali</t>
+  </si>
+  <si>
+    <t>Vinayak Mali</t>
+  </si>
+  <si>
+    <t>Prathmesh Killedar</t>
+  </si>
+  <si>
+    <t>Krishna Ware</t>
+  </si>
+  <si>
+    <t>Satish Wakde</t>
   </si>
 </sst>
 </file>
@@ -201,7 +207,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-14009]dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-14009]yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -246,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -254,6 +260,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -569,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577CAE7D-1992-4243-8BD9-FF0D62929D0C}">
-  <dimension ref="A1:AD5"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,12 +613,10 @@
     <col min="25" max="25" width="36.77734375" customWidth="1"/>
     <col min="26" max="26" width="29.88671875" customWidth="1"/>
     <col min="27" max="27" width="21.33203125" customWidth="1"/>
-    <col min="28" max="28" width="22.21875" customWidth="1"/>
-    <col min="29" max="29" width="20" customWidth="1"/>
-    <col min="30" max="30" width="24.33203125" customWidth="1"/>
+    <col min="28" max="28" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="2" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" s="2" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -619,7 +626,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -694,49 +701,43 @@
       <c r="AB1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="2" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3">
-        <v>2011</v>
+        <v>4000</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="5">
-        <v>44486</v>
+        <v>55</v>
+      </c>
+      <c r="D2" s="6">
+        <v>44523</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="3">
+        <v>918574968574</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="H2" s="3">
-        <v>8574968574</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="K2" s="3">
         <v>10</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M2" s="3">
         <v>2</v>
@@ -745,90 +746,84 @@
         <v>748596415263</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="T2" s="4">
         <v>85749685967</v>
       </c>
       <c r="U2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Z2" s="3">
         <v>9657690018</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB2" s="3">
-        <v>100</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD2" s="3">
-        <v>100</v>
+        <v>41</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3">
-        <v>2012</v>
+        <v>4001</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="5">
+        <v>52</v>
+      </c>
+      <c r="D3" s="6">
         <v>44486</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H3" s="3">
         <v>8574968574</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K3" s="3">
         <v>10</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M3" s="3">
         <v>2</v>
@@ -837,90 +832,84 @@
         <v>748596415263</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="T3" s="4">
         <v>85749685967</v>
       </c>
       <c r="U3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Z3" s="3">
         <v>9657690018</v>
       </c>
       <c r="AA3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB3" s="3">
-        <v>100</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD3" s="3">
-        <v>100</v>
+        <v>41</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3">
-        <v>2013</v>
+        <v>4002</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="5">
+        <v>53</v>
+      </c>
+      <c r="D4" s="6">
         <v>44486</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H4" s="3">
         <v>8574968574</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K4" s="3">
         <v>10</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M4" s="3">
         <v>2</v>
@@ -929,90 +918,84 @@
         <v>748596415263</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="T4" s="4">
         <v>85749685967</v>
       </c>
       <c r="U4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Z4" s="3">
         <v>9657690018</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB4" s="3">
-        <v>100</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD4" s="3">
-        <v>100</v>
+        <v>41</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" s="3">
-        <v>2014</v>
+        <v>4003</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="5">
+        <v>54</v>
+      </c>
+      <c r="D5" s="6">
         <v>44486</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H5" s="3">
         <v>8574968574</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K5" s="3">
         <v>10</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M5" s="3">
         <v>2</v>
@@ -1021,52 +1004,46 @@
         <v>748596415263</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="T5" s="4">
         <v>85749685967</v>
       </c>
       <c r="U5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="V5" s="3" t="s">
+      <c r="Y5" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="W5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y5" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Z5" s="3">
         <v>9657690018</v>
       </c>
       <c r="AA5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB5" s="3">
-        <v>100</v>
-      </c>
-      <c r="AC5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD5" s="3">
-        <v>100</v>
+        <v>41</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>